<commit_message>
add lines of code
</commit_message>
<xml_diff>
--- a/evaluation/experiment/data.xlsx
+++ b/evaluation/experiment/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gallushuber/git_proj/Huber.ER2CDS/evaluation/experiment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gallushuber/git_proj/ER2CDS/evaluation/experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CB4007-DAAC-6443-B88A-034FCD2345A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDB1AB8-3674-9A43-B22D-31784921A806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="700" windowWidth="45000" windowHeight="22840" xr2:uid="{AB73C851-2570-4848-9E24-9A6016711A1A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="172">
   <si>
     <t>/DMO/I_Travel_D</t>
   </si>
@@ -551,6 +551,9 @@
   </si>
   <si>
     <t>Std. Deviation</t>
+  </si>
+  <si>
+    <t>Lines of Code</t>
   </si>
 </sst>
 </file>
@@ -816,64 +819,64 @@
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>I_ACMSettlmtCtnHdrCostRevCkpt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>I_BkPOABankAccount</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>I_BPRelshpCntctPersnEmlAddrTP</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>I_BusPartMobileNumberGovTP</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>I_FieldLogisticsSupplier</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>I_FinSubstitutionRuleSubstnTP</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>I_MDOFIELD</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>I_MobileUserSession</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>I_ProdnRtgOperationTP</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>I_SourcingProject</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Z_I_AUSSENLAGER</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Z_I_BESTELLANFORDERUNG</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Z_I_CHANGEDOCUMENTITEM</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Z_I_DELIVANALYSIS</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>Z_I_MKPF</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>Z_I_BESTELLANFORDERUNG</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="15">
+                  <c:v>Z_I_Notification</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Z_I_PRODUCTION</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Z_I_PURCHDOCBASE</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Z_I_SDSERIALNUMBER</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Z_I_SERIALNMBRDELIVERY</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Z_I_CHANGEDOCUMENTITEM</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Z_I_DELIVANALYSIS</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Z_I_PRODUCTION</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Z_I_PURCHDOCBASE</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Z_I_AUSSENLAGER</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Z_I_SDSERIALNUMBER</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Z_I_Notification</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>I_ACMSettlmtCtnHdrCostRevCkpt</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>I_MobileUserSession</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>I_MDOFIELD</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>I_FinSubstitutionRuleSubstnTP</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>I_FieldLogisticsSupplier</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>I_BkPOABankAccount</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>I_BusPartMobileNumberGovTP</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>I_BPRelshpCntctPersnEmlAddrTP</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>I_ProdnRtgOperationTP</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>I_SourcingProject</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -885,52 +888,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>4</c:v>
@@ -939,10 +942,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>23</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6355,12 +6358,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E073B26E-32AF-5C4E-B08C-DB3284897244}" name="Table2" displayName="Table2" ref="A1:F21" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:F21" xr:uid="{E073B26E-32AF-5C4E-B08C-DB3284897244}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E073B26E-32AF-5C4E-B08C-DB3284897244}" name="Table2" displayName="Table2" ref="A1:G21" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:G21" xr:uid="{E073B26E-32AF-5C4E-B08C-DB3284897244}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G21">
+    <sortCondition ref="A1:A21"/>
+  </sortState>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{F9DADB49-9E36-4445-8133-ABDB69FA8F28}" name="Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{613C137D-B3C7-D04E-9099-6B9913178B57}" name="Relations"/>
     <tableColumn id="7" xr3:uid="{F8378F5E-1B23-044B-BCCF-413DF1BCC0A9}" name="Elements"/>
+    <tableColumn id="8" xr3:uid="{E55C92D7-31C0-0A49-8359-23FFB5FC7A52}" name="Lines of Code"/>
     <tableColumn id="3" xr3:uid="{A224C5CE-8087-2248-919C-820DCD052F2A}" name="Syntax"/>
     <tableColumn id="4" xr3:uid="{84D5766F-5980-E54C-924A-B5E993FA9B1F}" name="Output"/>
     <tableColumn id="6" xr3:uid="{015383A4-202E-814F-96B5-E37F45DDEB57}" name="Text"/>
@@ -6370,15 +6377,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A52FD4B8-3A75-5E40-B40C-6E4C40558033}" name="Table1" displayName="Table1" ref="A1:H101" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:H101" xr:uid="{A52FD4B8-3A75-5E40-B40C-6E4C40558033}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A52FD4B8-3A75-5E40-B40C-6E4C40558033}" name="Table1" displayName="Table1" ref="A1:I101" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:I101" xr:uid="{A52FD4B8-3A75-5E40-B40C-6E4C40558033}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I101">
     <sortCondition ref="A1:A101"/>
   </sortState>
-  <tableColumns count="8">
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0E2B2ADD-75B5-8545-AD31-04FADB27DD24}" name="Name" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{D671539F-52F9-9147-AEF6-776A08EE1F44}" name="Relations"/>
     <tableColumn id="3" xr3:uid="{18A5DAFF-5C5B-3D47-B1C0-95E4A95C54E0}" name="Elements"/>
+    <tableColumn id="9" xr3:uid="{503635CE-B351-B545-8623-ED9CCB4C1B1C}" name="Lines of Code"/>
     <tableColumn id="4" xr3:uid="{69016DE4-947B-2B47-B3DE-46C2664BB110}" name="Imported"/>
     <tableColumn id="5" xr3:uid="{16125078-5F1D-4C43-A141-CEC152CE33BB}" name="Display"/>
     <tableColumn id="6" xr3:uid="{3BCAC806-70E9-8B40-B033-98A78B0476C2}" name="Text"/>
@@ -6706,21 +6714,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4672D2B8-471A-1F4B-AB68-DDF5C0CFA150}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="88.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="88.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>83</v>
       </c>
@@ -6730,440 +6739,522 @@
       <c r="C1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>128</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>93</v>
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>17</v>
       </c>
       <c r="E2" t="s">
         <v>93</v>
       </c>
-      <c r="I2" t="s">
+      <c r="F2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" t="s">
+        <v>152</v>
+      </c>
+      <c r="J2" t="s">
         <v>84</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <f>MIN(Table2[Relations])</f>
         <v>0</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <f>MAX(Table2[Relations])</f>
         <v>23</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <f>AVERAGE(Table2[Relations])</f>
         <v>5.55</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <f>STDEV(Table2[Relations])</f>
         <v>6.1170598372610003</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>134</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>70</v>
-      </c>
-      <c r="D3" t="s">
-        <v>93</v>
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>33</v>
       </c>
       <c r="E3" t="s">
         <v>93</v>
       </c>
       <c r="F3" t="s">
-        <v>150</v>
-      </c>
-      <c r="I3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" t="s">
+        <v>149</v>
+      </c>
+      <c r="J3" t="s">
         <v>90</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <f>MIN(Table2[Elements])</f>
         <v>3</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <f>MAX(Table2[Elements])</f>
         <v>128</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <f>AVERAGE(Table2[Elements])</f>
         <v>31.05</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <f>STDEV(Table2[Elements])</f>
         <v>30.787001700136546</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" t="s">
+        <v>137</v>
+      </c>
+      <c r="J4" t="s">
+        <v>171</v>
+      </c>
+      <c r="K4">
+        <f>MIN(Table2[Lines of Code])</f>
+        <v>16</v>
+      </c>
+      <c r="L4">
+        <f>MAX(Table2[Lines of Code])</f>
+        <v>221</v>
+      </c>
+      <c r="M4">
+        <f>AVERAGE(Table2[Lines of Code])</f>
+        <v>65.3</v>
+      </c>
+      <c r="N4">
+        <f>STDEV(Table2[Lines of Code])</f>
+        <v>53.505631774411818</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="C7">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="E8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>128</v>
+      </c>
+      <c r="D10">
+        <v>147</v>
+      </c>
+      <c r="E10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>69</v>
+      </c>
+      <c r="D11">
+        <v>165</v>
+      </c>
+      <c r="E11" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
         <v>19</v>
       </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E8" t="s">
-        <v>93</v>
-      </c>
-      <c r="F8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="D12">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B11">
-        <v>19</v>
-      </c>
-      <c r="C11">
-        <v>70</v>
-      </c>
-      <c r="D11" t="s">
-        <v>93</v>
-      </c>
-      <c r="E11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>93</v>
-      </c>
-      <c r="E12" t="s">
-        <v>93</v>
-      </c>
-      <c r="F12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>129</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s">
-        <v>93</v>
+        <v>70</v>
+      </c>
+      <c r="D13">
+        <v>86</v>
       </c>
       <c r="E13" t="s">
         <v>93</v>
       </c>
       <c r="F13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+      <c r="G13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>93</v>
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>39</v>
       </c>
       <c r="E14" t="s">
         <v>93</v>
       </c>
       <c r="F14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>131</v>
+        <v>19</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s">
-        <v>93</v>
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>42</v>
       </c>
       <c r="E15" t="s">
         <v>93</v>
       </c>
       <c r="F15" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>132</v>
+        <v>18</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>18</v>
-      </c>
-      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16">
+        <v>39</v>
+      </c>
+      <c r="E16" t="s">
         <v>93</v>
       </c>
       <c r="F16" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C17">
-        <v>13</v>
-      </c>
-      <c r="D17" t="s">
-        <v>93</v>
+        <v>70</v>
+      </c>
+      <c r="D17">
+        <v>221</v>
       </c>
       <c r="E17" t="s">
         <v>93</v>
       </c>
       <c r="F17" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>135</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>4</v>
       </c>
       <c r="C18">
-        <v>19</v>
-      </c>
-      <c r="D18" t="s">
-        <v>93</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="D18">
+        <v>70</v>
+      </c>
+      <c r="E18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>136</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19">
-        <v>17</v>
-      </c>
-      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19">
+        <v>47</v>
+      </c>
+      <c r="E19" t="s">
         <v>93</v>
       </c>
       <c r="F19" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+      <c r="G19" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>140</v>
+        <v>23</v>
       </c>
       <c r="B20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C20">
-        <v>128</v>
-      </c>
-      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20">
+        <v>88</v>
+      </c>
+      <c r="E20" t="s">
         <v>93</v>
       </c>
       <c r="F20" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+      <c r="G20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B21">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C21">
-        <v>69</v>
-      </c>
-      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>21</v>
+      </c>
+      <c r="E21" t="s">
         <v>93</v>
       </c>
       <c r="F21" t="s">
-        <v>139</v>
+        <v>93</v>
+      </c>
+      <c r="G21" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -7176,24 +7267,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F650F4-ED0B-E44F-A328-2BD491C06275}">
-  <dimension ref="A1:O101"/>
+  <dimension ref="A1:P101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="6" max="6" width="60.1640625" customWidth="1"/>
-    <col min="7" max="7" width="85.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="7" max="7" width="60.1640625" customWidth="1"/>
+    <col min="8" max="8" width="85.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>83</v>
       </c>
@@ -7203,38 +7295,41 @@
       <c r="C1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -7244,33 +7339,36 @@
       <c r="C2">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>93</v>
+      <c r="D2">
+        <v>57</v>
       </c>
       <c r="E2" t="s">
         <v>93</v>
       </c>
-      <c r="K2" t="s">
+      <c r="F2" t="s">
+        <v>93</v>
+      </c>
+      <c r="L2" t="s">
         <v>84</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <f>MIN(Table1[Relations])</f>
         <v>0</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <f>MAX(Table1[Relations])</f>
         <v>30</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <f>AVERAGE(Table1[Relations])</f>
         <v>3.89</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <f>STDEV(Table1[Relations])</f>
         <v>4.9967565237437537</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -7280,33 +7378,36 @@
       <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
-        <v>93</v>
+      <c r="D3">
+        <v>51</v>
       </c>
       <c r="E3" t="s">
         <v>93</v>
       </c>
-      <c r="K3" t="s">
+      <c r="F3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L3" t="s">
         <v>90</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <f>MIN(Table1[Elements])</f>
         <v>2</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <f>MAX(Table1[Elements])</f>
         <v>325</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <f>AVERAGE(Table1[Elements])</f>
         <v>34.380000000000003</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <f>STDEV(Table1[Elements])</f>
         <v>49.347414042959464</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -7316,14 +7417,36 @@
       <c r="C4">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
-        <v>93</v>
+      <c r="D4">
+        <v>67</v>
       </c>
       <c r="E4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>93</v>
+      </c>
+      <c r="L4" t="s">
+        <v>171</v>
+      </c>
+      <c r="M4">
+        <f>MIN(Table1[Lines of Code])</f>
+        <v>31</v>
+      </c>
+      <c r="N4">
+        <f>MAX(Table1[Lines of Code])</f>
+        <v>1115</v>
+      </c>
+      <c r="O4">
+        <f>AVERAGE(Table1[Lines of Code])</f>
+        <v>116.76</v>
+      </c>
+      <c r="P4">
+        <f>STDEV(Table1[Lines of Code])</f>
+        <v>132.4048825734645</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -7333,14 +7456,17 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
-        <v>93</v>
+      <c r="D5">
+        <v>42</v>
       </c>
       <c r="E5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -7350,14 +7476,17 @@
       <c r="C6">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
-        <v>93</v>
+      <c r="D6">
+        <v>46</v>
       </c>
       <c r="E6" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -7367,14 +7496,17 @@
       <c r="C7">
         <v>12</v>
       </c>
-      <c r="D7" t="s">
-        <v>93</v>
+      <c r="D7">
+        <v>56</v>
       </c>
       <c r="E7" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -7384,14 +7516,17 @@
       <c r="C8">
         <v>9</v>
       </c>
-      <c r="D8" t="s">
-        <v>93</v>
+      <c r="D8">
+        <v>50</v>
       </c>
       <c r="E8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -7401,14 +7536,17 @@
       <c r="C9">
         <v>9</v>
       </c>
-      <c r="D9" t="s">
-        <v>93</v>
+      <c r="D9">
+        <v>61</v>
       </c>
       <c r="E9" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -7418,14 +7556,17 @@
       <c r="C10">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
-        <v>93</v>
+      <c r="D10">
+        <v>64</v>
       </c>
       <c r="E10" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -7435,14 +7576,17 @@
       <c r="C11">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
-        <v>93</v>
+      <c r="D11">
+        <v>65</v>
       </c>
       <c r="E11" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -7452,14 +7596,17 @@
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="D12" t="s">
-        <v>93</v>
+      <c r="D12">
+        <v>42</v>
       </c>
       <c r="E12" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -7469,14 +7616,17 @@
       <c r="C13">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
-        <v>93</v>
+      <c r="D13">
+        <v>46</v>
       </c>
       <c r="E13" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -7486,14 +7636,17 @@
       <c r="C14">
         <v>2</v>
       </c>
-      <c r="D14" t="s">
-        <v>93</v>
+      <c r="D14">
+        <v>42</v>
       </c>
       <c r="E14" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -7503,14 +7656,17 @@
       <c r="C15">
         <v>4</v>
       </c>
-      <c r="D15" t="s">
-        <v>93</v>
+      <c r="D15">
+        <v>47</v>
       </c>
       <c r="E15" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -7520,14 +7676,17 @@
       <c r="C16">
         <v>6</v>
       </c>
-      <c r="D16" t="s">
-        <v>93</v>
+      <c r="D16">
+        <v>50</v>
       </c>
       <c r="E16" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -7537,14 +7696,17 @@
       <c r="C17">
         <v>21</v>
       </c>
-      <c r="D17" t="s">
-        <v>93</v>
+      <c r="D17">
+        <v>74</v>
       </c>
       <c r="E17" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -7554,14 +7716,17 @@
       <c r="C18">
         <v>2</v>
       </c>
-      <c r="D18" t="s">
-        <v>93</v>
+      <c r="D18">
+        <v>42</v>
       </c>
       <c r="E18" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -7571,14 +7736,17 @@
       <c r="C19">
         <v>4</v>
       </c>
-      <c r="D19" t="s">
-        <v>93</v>
+      <c r="D19">
+        <v>46</v>
       </c>
       <c r="E19" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>74</v>
       </c>
@@ -7588,14 +7756,17 @@
       <c r="C20">
         <v>53</v>
       </c>
-      <c r="D20" t="s">
-        <v>93</v>
+      <c r="D20">
+        <v>119</v>
       </c>
       <c r="E20" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
@@ -7605,14 +7776,17 @@
       <c r="C21">
         <v>40</v>
       </c>
-      <c r="D21" t="s">
-        <v>93</v>
+      <c r="D21">
+        <v>89</v>
       </c>
       <c r="E21" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>70</v>
       </c>
@@ -7622,14 +7796,17 @@
       <c r="C22">
         <v>22</v>
       </c>
-      <c r="D22" t="s">
-        <v>93</v>
+      <c r="D22">
+        <v>80</v>
       </c>
       <c r="E22" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>78</v>
       </c>
@@ -7639,14 +7816,17 @@
       <c r="C23">
         <v>25</v>
       </c>
-      <c r="D23" t="s">
-        <v>93</v>
+      <c r="D23">
+        <v>69</v>
       </c>
       <c r="E23" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>69</v>
       </c>
@@ -7656,14 +7836,17 @@
       <c r="C24">
         <v>66</v>
       </c>
-      <c r="D24" t="s">
-        <v>93</v>
+      <c r="D24">
+        <v>173</v>
       </c>
       <c r="E24" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>73</v>
       </c>
@@ -7673,14 +7856,17 @@
       <c r="C25">
         <v>29</v>
       </c>
-      <c r="D25" t="s">
-        <v>93</v>
+      <c r="D25">
+        <v>105</v>
       </c>
       <c r="E25" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>77</v>
       </c>
@@ -7690,14 +7876,17 @@
       <c r="C26">
         <v>143</v>
       </c>
-      <c r="D26" t="s">
-        <v>93</v>
+      <c r="D26">
+        <v>218</v>
       </c>
       <c r="E26" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>76</v>
       </c>
@@ -7707,14 +7896,17 @@
       <c r="C27">
         <v>49</v>
       </c>
-      <c r="D27" t="s">
-        <v>93</v>
+      <c r="D27">
+        <v>85</v>
       </c>
       <c r="E27" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>81</v>
       </c>
@@ -7724,14 +7916,17 @@
       <c r="C28">
         <v>34</v>
       </c>
-      <c r="D28" t="s">
-        <v>93</v>
+      <c r="D28">
+        <v>79</v>
       </c>
       <c r="E28" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>79</v>
       </c>
@@ -7741,14 +7936,17 @@
       <c r="C29">
         <v>22</v>
       </c>
-      <c r="D29" t="s">
-        <v>93</v>
+      <c r="D29">
+        <v>65</v>
       </c>
       <c r="E29" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>71</v>
       </c>
@@ -7758,20 +7956,23 @@
       <c r="C30">
         <v>28</v>
       </c>
-      <c r="D30" t="s">
-        <v>93</v>
+      <c r="D30">
+        <v>121</v>
       </c>
       <c r="E30" t="s">
         <v>93</v>
       </c>
       <c r="F30" t="s">
+        <v>93</v>
+      </c>
+      <c r="G30" t="s">
         <v>97</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>75</v>
       </c>
@@ -7781,14 +7982,17 @@
       <c r="C31">
         <v>26</v>
       </c>
-      <c r="D31" t="s">
-        <v>93</v>
+      <c r="D31">
+        <v>104</v>
       </c>
       <c r="E31" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>82</v>
       </c>
@@ -7798,14 +8002,17 @@
       <c r="C32">
         <v>15</v>
       </c>
-      <c r="D32" t="s">
-        <v>93</v>
+      <c r="D32">
+        <v>67</v>
       </c>
       <c r="E32" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>80</v>
       </c>
@@ -7815,14 +8022,17 @@
       <c r="C33">
         <v>53</v>
       </c>
-      <c r="D33" t="s">
-        <v>93</v>
+      <c r="D33">
+        <v>119</v>
       </c>
       <c r="E33" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
@@ -7832,14 +8042,17 @@
       <c r="C34">
         <v>20</v>
       </c>
-      <c r="D34" t="s">
-        <v>93</v>
+      <c r="D34">
+        <v>75</v>
       </c>
       <c r="E34" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>59</v>
       </c>
@@ -7849,17 +8062,20 @@
       <c r="C35">
         <v>12</v>
       </c>
-      <c r="D35" t="s">
-        <v>93</v>
+      <c r="D35">
+        <v>59</v>
       </c>
       <c r="E35" t="s">
         <v>93</v>
       </c>
-      <c r="G35" t="s">
+      <c r="F35" t="s">
+        <v>93</v>
+      </c>
+      <c r="H35" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>60</v>
       </c>
@@ -7869,14 +8085,17 @@
       <c r="C36">
         <v>10</v>
       </c>
-      <c r="D36" t="s">
-        <v>93</v>
+      <c r="D36">
+        <v>52</v>
       </c>
       <c r="E36" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>61</v>
       </c>
@@ -7886,20 +8105,23 @@
       <c r="C37">
         <v>15</v>
       </c>
-      <c r="D37" t="s">
-        <v>93</v>
+      <c r="D37">
+        <v>71</v>
       </c>
       <c r="E37" t="s">
         <v>93</v>
       </c>
       <c r="F37" t="s">
+        <v>93</v>
+      </c>
+      <c r="G37" t="s">
         <v>100</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>126</v>
       </c>
@@ -7909,17 +8131,20 @@
       <c r="C38">
         <v>140</v>
       </c>
-      <c r="D38" t="s">
-        <v>93</v>
+      <c r="D38">
+        <v>1115</v>
       </c>
       <c r="E38" t="s">
         <v>93</v>
       </c>
       <c r="F38" t="s">
+        <v>93</v>
+      </c>
+      <c r="G38" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>55</v>
       </c>
@@ -7929,14 +8154,17 @@
       <c r="C39">
         <v>30</v>
       </c>
-      <c r="D39" t="s">
-        <v>93</v>
+      <c r="D39">
+        <v>218</v>
       </c>
       <c r="E39" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>49</v>
       </c>
@@ -7946,14 +8174,17 @@
       <c r="C40">
         <v>79</v>
       </c>
-      <c r="D40" t="s">
-        <v>93</v>
+      <c r="D40">
+        <v>185</v>
       </c>
       <c r="E40" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>48</v>
       </c>
@@ -7963,14 +8194,17 @@
       <c r="C41">
         <v>42</v>
       </c>
-      <c r="D41" t="s">
-        <v>93</v>
+      <c r="D41">
+        <v>151</v>
       </c>
       <c r="E41" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F41" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>54</v>
       </c>
@@ -7980,20 +8214,23 @@
       <c r="C42">
         <v>21</v>
       </c>
-      <c r="D42" t="s">
-        <v>93</v>
+      <c r="D42">
+        <v>117</v>
       </c>
       <c r="E42" t="s">
         <v>93</v>
       </c>
       <c r="F42" t="s">
+        <v>93</v>
+      </c>
+      <c r="G42" t="s">
         <v>162</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>51</v>
       </c>
@@ -8003,14 +8240,17 @@
       <c r="C43">
         <v>22</v>
       </c>
-      <c r="D43" t="s">
-        <v>93</v>
+      <c r="D43">
+        <v>138</v>
       </c>
       <c r="E43" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>62</v>
       </c>
@@ -8020,14 +8260,17 @@
       <c r="C44">
         <v>11</v>
       </c>
-      <c r="D44" t="s">
-        <v>93</v>
+      <c r="D44">
+        <v>51</v>
       </c>
       <c r="E44" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>63</v>
       </c>
@@ -8037,14 +8280,17 @@
       <c r="C45">
         <v>66</v>
       </c>
-      <c r="D45" t="s">
-        <v>93</v>
+      <c r="D45">
+        <v>534</v>
       </c>
       <c r="E45" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>52</v>
       </c>
@@ -8054,14 +8300,17 @@
       <c r="C46">
         <v>32</v>
       </c>
-      <c r="D46" t="s">
-        <v>93</v>
+      <c r="D46">
+        <v>156</v>
       </c>
       <c r="E46" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>56</v>
       </c>
@@ -8071,14 +8320,17 @@
       <c r="C47">
         <v>16</v>
       </c>
-      <c r="D47" t="s">
-        <v>93</v>
+      <c r="D47">
+        <v>121</v>
       </c>
       <c r="E47" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>50</v>
       </c>
@@ -8088,20 +8340,23 @@
       <c r="C48">
         <v>36</v>
       </c>
-      <c r="D48" t="s">
-        <v>93</v>
+      <c r="D48">
+        <v>224</v>
       </c>
       <c r="E48" t="s">
         <v>93</v>
       </c>
       <c r="F48" t="s">
+        <v>93</v>
+      </c>
+      <c r="G48" t="s">
         <v>97</v>
       </c>
-      <c r="H48" t="s">
+      <c r="I48" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
@@ -8111,20 +8366,23 @@
       <c r="C49">
         <v>38</v>
       </c>
-      <c r="D49" t="s">
-        <v>93</v>
+      <c r="D49">
+        <v>206</v>
       </c>
       <c r="E49" t="s">
         <v>93</v>
       </c>
       <c r="F49" t="s">
+        <v>93</v>
+      </c>
+      <c r="G49" t="s">
         <v>97</v>
       </c>
-      <c r="H49" t="s">
+      <c r="I49" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>64</v>
       </c>
@@ -8134,14 +8392,17 @@
       <c r="C50">
         <v>16</v>
       </c>
-      <c r="D50" t="s">
-        <v>93</v>
+      <c r="D50">
+        <v>70</v>
       </c>
       <c r="E50" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F50" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>57</v>
       </c>
@@ -8151,14 +8412,17 @@
       <c r="C51">
         <v>14</v>
       </c>
-      <c r="D51" t="s">
-        <v>93</v>
+      <c r="D51">
+        <v>78</v>
       </c>
       <c r="E51" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>65</v>
       </c>
@@ -8168,14 +8432,17 @@
       <c r="C52">
         <v>8</v>
       </c>
-      <c r="D52" t="s">
-        <v>93</v>
+      <c r="D52">
+        <v>61</v>
       </c>
       <c r="E52" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F52" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>66</v>
       </c>
@@ -8185,14 +8452,17 @@
       <c r="C53">
         <v>9</v>
       </c>
-      <c r="D53" t="s">
-        <v>93</v>
+      <c r="D53">
+        <v>59</v>
       </c>
       <c r="E53" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F53" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>67</v>
       </c>
@@ -8202,14 +8472,17 @@
       <c r="C54">
         <v>17</v>
       </c>
-      <c r="D54" t="s">
-        <v>93</v>
+      <c r="D54">
+        <v>69</v>
       </c>
       <c r="E54" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F54" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>68</v>
       </c>
@@ -8219,14 +8492,17 @@
       <c r="C55">
         <v>8</v>
       </c>
-      <c r="D55" t="s">
-        <v>93</v>
+      <c r="D55">
+        <v>56</v>
       </c>
       <c r="E55" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F55" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>24</v>
       </c>
@@ -8236,14 +8512,17 @@
       <c r="C56">
         <v>4</v>
       </c>
-      <c r="D56" t="s">
-        <v>93</v>
+      <c r="D56">
+        <v>36</v>
       </c>
       <c r="E56" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F56" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>25</v>
       </c>
@@ -8253,14 +8532,17 @@
       <c r="C57">
         <v>11</v>
       </c>
-      <c r="D57" t="s">
-        <v>93</v>
+      <c r="D57">
+        <v>49</v>
       </c>
       <c r="E57" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F57" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>26</v>
       </c>
@@ -8270,14 +8552,17 @@
       <c r="C58">
         <v>14</v>
       </c>
-      <c r="D58" t="s">
-        <v>93</v>
+      <c r="D58">
+        <v>49</v>
       </c>
       <c r="E58" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F58" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>27</v>
       </c>
@@ -8287,14 +8572,17 @@
       <c r="C59">
         <v>5</v>
       </c>
-      <c r="D59" t="s">
-        <v>93</v>
+      <c r="D59">
+        <v>41</v>
       </c>
       <c r="E59" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F59" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>28</v>
       </c>
@@ -8304,14 +8592,17 @@
       <c r="C60">
         <v>38</v>
       </c>
-      <c r="D60" t="s">
-        <v>93</v>
+      <c r="D60">
+        <v>108</v>
       </c>
       <c r="E60" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F60" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>29</v>
       </c>
@@ -8321,14 +8612,17 @@
       <c r="C61">
         <v>17</v>
       </c>
-      <c r="D61" t="s">
-        <v>93</v>
+      <c r="D61">
+        <v>79</v>
       </c>
       <c r="E61" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F61" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>35</v>
       </c>
@@ -8338,14 +8632,17 @@
       <c r="C62">
         <v>70</v>
       </c>
-      <c r="D62" t="s">
-        <v>93</v>
+      <c r="D62">
+        <v>134</v>
       </c>
       <c r="E62" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F62" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>36</v>
       </c>
@@ -8355,20 +8652,23 @@
       <c r="C63">
         <v>122</v>
       </c>
-      <c r="D63" t="s">
-        <v>93</v>
+      <c r="D63">
+        <v>269</v>
       </c>
       <c r="E63" t="s">
         <v>93</v>
       </c>
       <c r="F63" t="s">
+        <v>93</v>
+      </c>
+      <c r="G63" t="s">
         <v>94</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>39</v>
       </c>
@@ -8378,14 +8678,17 @@
       <c r="C64">
         <v>5</v>
       </c>
-      <c r="D64" t="s">
-        <v>93</v>
+      <c r="D64">
+        <v>54</v>
       </c>
       <c r="E64" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F64" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>45</v>
       </c>
@@ -8395,14 +8698,17 @@
       <c r="C65">
         <v>4</v>
       </c>
-      <c r="D65" t="s">
-        <v>93</v>
+      <c r="D65">
+        <v>55</v>
       </c>
       <c r="E65" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F65" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>37</v>
       </c>
@@ -8412,14 +8718,17 @@
       <c r="C66">
         <v>4</v>
       </c>
-      <c r="D66" t="s">
-        <v>93</v>
+      <c r="D66">
+        <v>56</v>
       </c>
       <c r="E66" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F66" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>46</v>
       </c>
@@ -8429,14 +8738,17 @@
       <c r="C67">
         <v>4</v>
       </c>
-      <c r="D67" t="s">
-        <v>93</v>
+      <c r="D67">
+        <v>55</v>
       </c>
       <c r="E67" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F67" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>32</v>
       </c>
@@ -8446,14 +8758,17 @@
       <c r="C68">
         <v>12</v>
       </c>
-      <c r="D68" t="s">
-        <v>93</v>
+      <c r="D68">
+        <v>152</v>
       </c>
       <c r="E68" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F68" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>47</v>
       </c>
@@ -8463,14 +8778,17 @@
       <c r="C69">
         <v>3</v>
       </c>
-      <c r="D69" t="s">
-        <v>93</v>
+      <c r="D69">
+        <v>51</v>
       </c>
       <c r="E69" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F69" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>40</v>
       </c>
@@ -8480,14 +8798,17 @@
       <c r="C70">
         <v>5</v>
       </c>
-      <c r="D70" t="s">
-        <v>93</v>
+      <c r="D70">
+        <v>51</v>
       </c>
       <c r="E70" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F70" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>42</v>
       </c>
@@ -8497,14 +8818,17 @@
       <c r="C71">
         <v>37</v>
       </c>
-      <c r="D71" t="s">
-        <v>93</v>
+      <c r="D71">
+        <v>68</v>
       </c>
       <c r="E71" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F71" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>38</v>
       </c>
@@ -8514,14 +8838,17 @@
       <c r="C72">
         <v>8</v>
       </c>
-      <c r="D72" t="s">
-        <v>93</v>
+      <c r="D72">
+        <v>46</v>
       </c>
       <c r="E72" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F72" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>43</v>
       </c>
@@ -8531,14 +8858,17 @@
       <c r="C73">
         <v>2</v>
       </c>
-      <c r="D73" t="s">
-        <v>93</v>
+      <c r="D73">
+        <v>31</v>
       </c>
       <c r="E73" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F73" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>34</v>
       </c>
@@ -8548,14 +8878,17 @@
       <c r="C74">
         <v>10</v>
       </c>
-      <c r="D74" t="s">
-        <v>93</v>
+      <c r="D74">
+        <v>57</v>
       </c>
       <c r="E74" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F74" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>31</v>
       </c>
@@ -8565,14 +8898,17 @@
       <c r="C75">
         <v>89</v>
       </c>
-      <c r="D75" t="s">
-        <v>93</v>
+      <c r="D75">
+        <v>230</v>
       </c>
       <c r="E75" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F75" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>30</v>
       </c>
@@ -8582,14 +8918,17 @@
       <c r="C76">
         <v>52</v>
       </c>
-      <c r="D76" t="s">
-        <v>93</v>
+      <c r="D76">
+        <v>201</v>
       </c>
       <c r="E76" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F76" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>44</v>
       </c>
@@ -8599,14 +8938,17 @@
       <c r="C77">
         <v>2</v>
       </c>
-      <c r="D77" t="s">
-        <v>93</v>
+      <c r="D77">
+        <v>38</v>
       </c>
       <c r="E77" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F77" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>33</v>
       </c>
@@ -8616,14 +8958,17 @@
       <c r="C78">
         <v>132</v>
       </c>
-      <c r="D78" t="s">
-        <v>93</v>
+      <c r="D78">
+        <v>294</v>
       </c>
       <c r="E78" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F78" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>41</v>
       </c>
@@ -8633,17 +8978,20 @@
       <c r="C79">
         <v>29</v>
       </c>
-      <c r="D79" t="s">
-        <v>93</v>
+      <c r="D79">
+        <v>137</v>
       </c>
       <c r="E79" t="s">
         <v>93</v>
       </c>
       <c r="F79" t="s">
+        <v>93</v>
+      </c>
+      <c r="G79" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>119</v>
       </c>
@@ -8653,20 +9001,23 @@
       <c r="C80">
         <v>13</v>
       </c>
-      <c r="D80" t="s">
-        <v>93</v>
+      <c r="D80">
+        <v>62</v>
       </c>
       <c r="E80" t="s">
         <v>93</v>
       </c>
       <c r="F80" t="s">
+        <v>93</v>
+      </c>
+      <c r="G80" t="s">
         <v>100</v>
       </c>
-      <c r="H80" t="s">
+      <c r="I80" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>121</v>
       </c>
@@ -8676,14 +9027,17 @@
       <c r="C81">
         <v>20</v>
       </c>
-      <c r="D81" t="s">
-        <v>93</v>
+      <c r="D81">
+        <v>69</v>
       </c>
       <c r="E81" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F81" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>113</v>
       </c>
@@ -8693,17 +9047,20 @@
       <c r="C82">
         <v>167</v>
       </c>
-      <c r="D82" t="s">
-        <v>93</v>
+      <c r="D82">
+        <v>257</v>
       </c>
       <c r="E82" t="s">
         <v>93</v>
       </c>
       <c r="F82" t="s">
+        <v>93</v>
+      </c>
+      <c r="G82" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>122</v>
       </c>
@@ -8713,17 +9070,20 @@
       <c r="C83">
         <v>92</v>
       </c>
-      <c r="D83" t="s">
-        <v>93</v>
+      <c r="D83">
+        <v>206</v>
       </c>
       <c r="E83" t="s">
         <v>93</v>
       </c>
       <c r="F83" t="s">
+        <v>93</v>
+      </c>
+      <c r="G83" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>116</v>
       </c>
@@ -8733,17 +9093,20 @@
       <c r="C84">
         <v>6</v>
       </c>
-      <c r="D84" t="s">
-        <v>93</v>
+      <c r="D84">
+        <v>63</v>
       </c>
       <c r="E84" t="s">
         <v>93</v>
       </c>
       <c r="F84" t="s">
+        <v>93</v>
+      </c>
+      <c r="G84" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>115</v>
       </c>
@@ -8753,14 +9116,17 @@
       <c r="C85">
         <v>12</v>
       </c>
-      <c r="D85" t="s">
-        <v>93</v>
+      <c r="D85">
+        <v>116</v>
       </c>
       <c r="E85" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F85" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>124</v>
       </c>
@@ -8770,14 +9136,17 @@
       <c r="C86">
         <v>10</v>
       </c>
-      <c r="D86" t="s">
-        <v>93</v>
+      <c r="D86">
+        <v>51</v>
       </c>
       <c r="E86" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F86" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>125</v>
       </c>
@@ -8787,14 +9156,17 @@
       <c r="C87">
         <v>29</v>
       </c>
-      <c r="D87" t="s">
-        <v>93</v>
+      <c r="D87">
+        <v>71</v>
       </c>
       <c r="E87" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F87" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>123</v>
       </c>
@@ -8804,14 +9176,17 @@
       <c r="C88">
         <v>19</v>
       </c>
-      <c r="D88" t="s">
-        <v>93</v>
+      <c r="D88">
+        <v>90</v>
       </c>
       <c r="E88" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F88" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>118</v>
       </c>
@@ -8821,14 +9196,17 @@
       <c r="C89">
         <v>5</v>
       </c>
-      <c r="D89" t="s">
-        <v>93</v>
+      <c r="D89">
+        <v>63</v>
       </c>
       <c r="E89" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F89" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>114</v>
       </c>
@@ -8838,14 +9216,17 @@
       <c r="C90">
         <v>7</v>
       </c>
-      <c r="D90" t="s">
-        <v>93</v>
+      <c r="D90">
+        <v>72</v>
       </c>
       <c r="E90" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F90" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>112</v>
       </c>
@@ -8855,14 +9236,17 @@
       <c r="C91">
         <v>223</v>
       </c>
-      <c r="D91" t="s">
-        <v>93</v>
+      <c r="D91">
+        <v>340</v>
       </c>
       <c r="E91" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F91" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>101</v>
       </c>
@@ -8872,14 +9256,17 @@
       <c r="C92">
         <v>94</v>
       </c>
-      <c r="D92" t="s">
-        <v>93</v>
+      <c r="D92">
+        <v>176</v>
       </c>
       <c r="E92" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F92" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>111</v>
       </c>
@@ -8889,14 +9276,17 @@
       <c r="C93">
         <v>325</v>
       </c>
-      <c r="D93" t="s">
-        <v>93</v>
+      <c r="D93">
+        <v>477</v>
       </c>
       <c r="E93" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F93" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>109</v>
       </c>
@@ -8906,14 +9296,17 @@
       <c r="C94">
         <v>26</v>
       </c>
-      <c r="D94" t="s">
-        <v>93</v>
+      <c r="D94">
+        <v>126</v>
       </c>
       <c r="E94" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F94" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>108</v>
       </c>
@@ -8923,14 +9316,17 @@
       <c r="C95">
         <v>21</v>
       </c>
-      <c r="D95" t="s">
-        <v>93</v>
+      <c r="D95">
+        <v>114</v>
       </c>
       <c r="E95" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F95" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>107</v>
       </c>
@@ -8940,20 +9336,23 @@
       <c r="C96">
         <v>121</v>
       </c>
-      <c r="D96" t="s">
-        <v>93</v>
+      <c r="D96">
+        <v>193</v>
       </c>
       <c r="E96" t="s">
         <v>93</v>
       </c>
       <c r="F96" t="s">
+        <v>93</v>
+      </c>
+      <c r="G96" t="s">
         <v>110</v>
       </c>
-      <c r="H96" t="s">
+      <c r="I96" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>106</v>
       </c>
@@ -8963,14 +9362,17 @@
       <c r="C97">
         <v>21</v>
       </c>
-      <c r="D97" t="s">
-        <v>93</v>
+      <c r="D97">
+        <v>63</v>
       </c>
       <c r="E97" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>102</v>
       </c>
@@ -8980,14 +9382,17 @@
       <c r="C98">
         <v>60</v>
       </c>
-      <c r="D98" t="s">
-        <v>93</v>
+      <c r="D98">
+        <v>144</v>
       </c>
       <c r="E98" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>105</v>
       </c>
@@ -8997,14 +9402,17 @@
       <c r="C99">
         <v>5</v>
       </c>
-      <c r="D99" t="s">
-        <v>93</v>
+      <c r="D99">
+        <v>41</v>
       </c>
       <c r="E99" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>104</v>
       </c>
@@ -9014,14 +9422,17 @@
       <c r="C100">
         <v>44</v>
       </c>
-      <c r="D100" t="s">
-        <v>93</v>
+      <c r="D100">
+        <v>128</v>
       </c>
       <c r="E100" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>103</v>
       </c>
@@ -9031,10 +9442,13 @@
       <c r="C101">
         <v>36</v>
       </c>
-      <c r="D101" t="s">
-        <v>93</v>
+      <c r="D101">
+        <v>106</v>
       </c>
       <c r="E101" t="s">
+        <v>93</v>
+      </c>
+      <c r="F101" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>